<commit_message>
Build v2.1.4: Fix YAML anchor bug in OAS 3.0 headers - use deepcopy
</commit_message>
<xml_diff>
--- a/Templates Master/endpoint.xlsx
+++ b/Templates Master/endpoint.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr codeName="Questa_cartella_di_lavoro"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giuse\.gemini\antigravity\scratch\OASIS\Templates Master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311B4729-6E5F-416A-9AC5-BBD596C493B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05BB2DD-54DB-4BD9-ADBA-DB881A4C1A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -589,7 +589,7 @@
   </sheetPr>
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
@@ -805,7 +805,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,11 +834,11 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>

</xml_diff>